<commit_message>
Corrected and more fast method. Add and correct diagram.
</commit_message>
<xml_diff>
--- a/bin/4-MeO-Ph-N2+-MTMO-transform.xlsx
+++ b/bin/4-MeO-Ph-N2+-MTMO-transform.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="26">
   <si>
     <t xml:space="preserve">MinE_MO</t>
   </si>
@@ -94,16 +94,23 @@
   <si>
     <t xml:space="preserve">∑dE</t>
   </si>
+  <si>
+    <t xml:space="preserve">N2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-MeOPh+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,6 +135,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFB2B2B2"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -187,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,6 +230,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,6 +256,18 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -253,7 +295,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -305,10 +347,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H45" activeCellId="0" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1656,235 +1698,261 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="n">
+      <c r="A37" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="3" t="n">
+      <c r="B37" s="7" t="n">
         <v>-0.26947</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="7" t="n">
         <v>36</v>
       </c>
-      <c r="D37" s="3" t="n">
+      <c r="D37" s="7" t="n">
         <v>-0.22758</v>
       </c>
-      <c r="E37" s="3" t="n">
+      <c r="E37" s="7" t="n">
         <v>28</v>
       </c>
-      <c r="F37" s="3" t="n">
+      <c r="F37" s="7" t="n">
         <v>-0.336484</v>
       </c>
-      <c r="G37" s="3" t="n">
+      <c r="G37" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="3" t="s">
+      <c r="H37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="3" t="n">
+      <c r="J37" s="7" t="n">
         <f aca="false">B37-F37</f>
         <v>0.067014</v>
       </c>
-      <c r="K37" s="4"/>
+      <c r="K37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="A38" s="9" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="5" t="n">
+      <c r="B38" s="9" t="n">
         <v>-0.25866</v>
       </c>
-      <c r="C38" s="5" t="n">
+      <c r="C38" s="9" t="n">
         <v>41</v>
       </c>
-      <c r="D38" s="5" t="n">
+      <c r="D38" s="9" t="n">
         <v>-0.05683</v>
       </c>
-      <c r="E38" s="5" t="n">
+      <c r="E38" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="F38" s="5" t="n">
+      <c r="F38" s="9" t="n">
         <v>-0.022965</v>
       </c>
-      <c r="G38" s="5" t="n">
+      <c r="G38" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H38" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="I38" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J38" s="5" t="n">
+      <c r="J38" s="9" t="n">
         <f aca="false">B38-F38</f>
         <v>-0.235695</v>
       </c>
-      <c r="K38" s="6"/>
+      <c r="K38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="n">
+      <c r="A39" s="7" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="3" t="n">
+      <c r="B39" s="7" t="n">
         <v>-0.19089</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="7" t="n">
         <v>37</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="7" t="n">
         <v>-0.19946</v>
       </c>
-      <c r="E39" s="3" t="n">
+      <c r="E39" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" s="7" t="n">
         <v>-0.227596</v>
       </c>
-      <c r="G39" s="3" t="n">
+      <c r="G39" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="3" t="s">
+      <c r="H39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="3" t="n">
+      <c r="J39" s="7" t="n">
         <f aca="false">B39-F39</f>
         <v>0.036706</v>
       </c>
-      <c r="K39" s="4"/>
+      <c r="K39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
+      <c r="A40" s="9" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="5" t="n">
+      <c r="B40" s="9" t="n">
         <v>-0.15148</v>
       </c>
-      <c r="C40" s="5" t="n">
+      <c r="C40" s="9" t="n">
         <v>40</v>
       </c>
-      <c r="D40" s="5" t="n">
+      <c r="D40" s="9" t="n">
         <v>-0.05686</v>
       </c>
-      <c r="E40" s="5" t="n">
+      <c r="E40" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="F40" s="5" t="n">
+      <c r="F40" s="9" t="n">
         <v>-0.022962</v>
       </c>
-      <c r="G40" s="5" t="n">
+      <c r="G40" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="H40" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J40" s="5" t="n">
+      <c r="J40" s="9" t="n">
         <f aca="false">B40-F40</f>
         <v>-0.128518</v>
       </c>
-      <c r="K40" s="6"/>
+      <c r="K40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="n">
+      <c r="A41" s="7" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="3" t="n">
+      <c r="B41" s="7" t="n">
         <v>-0.08323</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="7" t="n">
         <v>-0.3362</v>
       </c>
-      <c r="E41" s="3" t="n">
+      <c r="E41" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" s="7" t="n">
         <v>-0.199599</v>
       </c>
-      <c r="G41" s="3" t="n">
+      <c r="G41" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I41" s="3" t="s">
+      <c r="H41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J41" s="3" t="n">
+      <c r="J41" s="7" t="n">
         <f aca="false">B41-F41</f>
         <v>0.116369</v>
       </c>
-      <c r="K41" s="4"/>
+      <c r="K41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="n">
+      <c r="A42" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="3" t="n">
+      <c r="B42" s="7" t="n">
         <v>-0.041</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="7" t="n">
         <v>38</v>
       </c>
-      <c r="D42" s="3" t="n">
+      <c r="D42" s="7" t="n">
         <v>-0.08471</v>
       </c>
-      <c r="E42" s="3" t="n">
+      <c r="E42" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="7" t="n">
         <v>-0.085089</v>
       </c>
-      <c r="G42" s="3" t="n">
+      <c r="G42" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="3" t="s">
+      <c r="H42" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="3" t="n">
+      <c r="J42" s="7" t="n">
         <f aca="false">B42-F42</f>
         <v>0.044089</v>
       </c>
-      <c r="K42" s="4"/>
+      <c r="K42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K43" s="7"/>
+      <c r="K43" s="11"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="8" t="n">
+      <c r="B44" s="12" t="n">
         <f aca="false">SUM(B1:B36)</f>
         <v>-140.03513</v>
       </c>
-      <c r="D44" s="8" t="n">
+      <c r="D44" s="12" t="n">
         <f aca="false">SUM(D1:D36)</f>
         <v>-139.12117</v>
       </c>
-      <c r="F44" s="8" t="n">
+      <c r="F44" s="12" t="n">
         <f aca="false">SUM(F1:F36)</f>
         <v>-138.857824</v>
       </c>
-      <c r="J44" s="8" t="n">
+      <c r="J44" s="12" t="n">
         <f aca="false">SUM(J2:J36)</f>
         <v>-1.177306</v>
       </c>
-      <c r="K44" s="9" t="n">
+      <c r="K44" s="13" t="n">
         <f aca="false">SUM(K2:K36)</f>
         <v>-100</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H45" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J45" s="15" t="n">
+        <f aca="false">J3+J4+J12+J20+J29+J30+J32</f>
+        <v>-1.243505</v>
+      </c>
+      <c r="K45" s="16" t="n">
+        <f aca="false">K3+K4+K12+K20+K29+K30+K32</f>
+        <v>-105.622922162972</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H46" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J46" s="15" t="n">
+        <f aca="false">SUM(J2,J5:J11,J13:J19,J21:J28,J31,J33:J36)</f>
+        <v>0.0661989999999951</v>
+      </c>
+      <c r="K46" s="16" t="n">
+        <f aca="false">SUM(K2,K5:K11,K13:K19,K21:K28,K31,K33:K36)</f>
+        <v>5.62292216297165</v>
       </c>
     </row>
   </sheetData>
@@ -1903,10 +1971,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1916,7 +1984,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.02"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2927,177 +2995,203 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="n">
+      <c r="A37" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="3" t="n">
+      <c r="B37" s="7" t="n">
         <v>-0.26947</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="7" t="n">
         <v>28</v>
       </c>
-      <c r="D37" s="3" t="n">
+      <c r="D37" s="7" t="n">
         <v>-0.336484</v>
       </c>
-      <c r="E37" s="3" t="n">
+      <c r="E37" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="3" t="n">
+      <c r="F37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="7" t="n">
         <f aca="false">B37-D37</f>
         <v>0.067014</v>
       </c>
-      <c r="H37" s="4"/>
+      <c r="H37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="A38" s="9" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="5" t="n">
+      <c r="B38" s="9" t="n">
         <v>-0.25866</v>
       </c>
-      <c r="C38" s="5" t="n">
+      <c r="C38" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="D38" s="5" t="n">
+      <c r="D38" s="9" t="n">
         <v>-0.022965</v>
       </c>
-      <c r="E38" s="5" t="n">
+      <c r="E38" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="5" t="n">
+      <c r="G38" s="9" t="n">
         <f aca="false">B38-D38</f>
         <v>-0.235695</v>
       </c>
-      <c r="H38" s="6"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="n">
+      <c r="A39" s="7" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="3" t="n">
+      <c r="B39" s="7" t="n">
         <v>-0.19089</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="7" t="n">
         <v>-0.227596</v>
       </c>
-      <c r="E39" s="3" t="n">
+      <c r="E39" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="3" t="n">
+      <c r="F39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="7" t="n">
         <f aca="false">B39-D39</f>
         <v>0.036706</v>
       </c>
-      <c r="H39" s="4"/>
+      <c r="H39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
+      <c r="A40" s="9" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="5" t="n">
+      <c r="B40" s="9" t="n">
         <v>-0.15148</v>
       </c>
-      <c r="C40" s="5" t="n">
+      <c r="C40" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="D40" s="5" t="n">
+      <c r="D40" s="9" t="n">
         <v>-0.022962</v>
       </c>
-      <c r="E40" s="5" t="n">
+      <c r="E40" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="5" t="n">
+      <c r="G40" s="9" t="n">
         <f aca="false">B40-D40</f>
         <v>-0.128518</v>
       </c>
-      <c r="H40" s="6"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="n">
+      <c r="A41" s="7" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="3" t="n">
+      <c r="B41" s="7" t="n">
         <v>-0.08323</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="7" t="n">
         <v>-0.199599</v>
       </c>
-      <c r="E41" s="3" t="n">
+      <c r="E41" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="3" t="n">
+      <c r="F41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="7" t="n">
         <f aca="false">B41-D41</f>
         <v>0.116369</v>
       </c>
-      <c r="H41" s="4"/>
+      <c r="H41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="n">
+      <c r="A42" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="3" t="n">
+      <c r="B42" s="7" t="n">
         <v>-0.041</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="D42" s="3" t="n">
+      <c r="D42" s="7" t="n">
         <v>-0.085089</v>
       </c>
-      <c r="E42" s="3" t="n">
+      <c r="E42" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="3" t="n">
+      <c r="F42" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="7" t="n">
         <f aca="false">B42-D42</f>
         <v>0.044089</v>
       </c>
-      <c r="H42" s="4"/>
+      <c r="H42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="7"/>
+      <c r="H43" s="11"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="8" t="n">
+      <c r="B44" s="12" t="n">
         <f aca="false">SUM(B1:B36)</f>
         <v>-140.03513</v>
       </c>
-      <c r="D44" s="8" t="n">
+      <c r="D44" s="12" t="n">
         <f aca="false">SUM(D1:D36)</f>
         <v>-138.857824</v>
       </c>
-      <c r="G44" s="8" t="n">
+      <c r="G44" s="12" t="n">
         <f aca="false">SUM(G2:G36)</f>
         <v>-1.177306</v>
       </c>
-      <c r="H44" s="9" t="n">
+      <c r="H44" s="13" t="n">
         <f aca="false">SUM(H2:H36)</f>
         <v>-100</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F45" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="15" t="n">
+        <f aca="false">G3+G4+G12+G20+G29+G30+G32</f>
+        <v>-1.243505</v>
+      </c>
+      <c r="H45" s="16" t="n">
+        <f aca="false">H3+H4+H12+H20+H29+H30+H32</f>
+        <v>-105.622922162972</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F46" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="15" t="n">
+        <f aca="false">SUM(G2,G5:G11,G13:G19,G21:G28,G31,G33:G36)</f>
+        <v>0.0661989999999951</v>
+      </c>
+      <c r="H46" s="16" t="n">
+        <f aca="false">SUM(H2,H5:H11,H13:H19,H21:H28,H31,H33:H36)</f>
+        <v>5.62292216297165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>